<commit_message>
Report: Update WTS and Report tab UI
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_10.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_10.xlsx
@@ -157,12 +157,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -220,18 +226,6 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -247,6 +241,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,7 +562,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="A4" sqref="A4:V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,100 +588,100 @@
     <col min="23" max="23" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I1" s="10" t="s">
+    <row r="1" spans="1:23" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I2" s="8" t="s">
+    <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="7" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:23" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="S4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="5"/>
+      <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
Home-Report: Report filter function added. Signatory option added. Common header footer added.
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_10.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_10.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$9:$9</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Withholding Taxes Summary Report</t>
   </si>
@@ -100,10 +100,13 @@
 Rate</t>
   </si>
   <si>
-    <t>&gt;</t>
-  </si>
-  <si>
-    <t>&lt;</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>TIN</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>
@@ -128,14 +131,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -151,6 +146,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -224,35 +226,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -269,6 +274,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>10026</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>10026</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>29904</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>131823</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10026" y="10026"/>
+          <a:ext cx="1010478" cy="312297"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,10 +613,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:V4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,111 +642,224 @@
     <col min="23" max="23" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I1" s="6" t="s">
+    <row r="1" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
     </row>
-    <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I2" s="4" t="s">
+    <row r="2" spans="1:23" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+    </row>
+    <row r="3" spans="1:23" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+    </row>
+    <row r="4" spans="1:23" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:23" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="5" spans="1:23" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+    </row>
+    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:23" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="P7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="Q7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="R7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="S7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="T7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="U7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="7" t="s">
+      <c r="V7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="1"/>
+      <c r="W7" s="1"/>
     </row>
-    <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
+    <row r="8" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="I1:N1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A2:V2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C3:V3"/>
+    <mergeCell ref="C4:V4"/>
+    <mergeCell ref="C5:V5"/>
   </mergeCells>
-  <pageMargins left="0.19675925925925927" right="0.12731481481481483" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.19675925925925927" right="0.12731481481481483" top="0.26041666666666669" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;D&amp;CPAGE =&gt; &amp;P of &amp;N</oddFooter>
+    <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>